<commit_message>
ya he localizado layyyers
</commit_message>
<xml_diff>
--- a/horas.xlsx
+++ b/horas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t xml:space="preserve">Fechas</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t xml:space="preserve">1-dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-dic</t>
   </si>
 </sst>
 </file>
@@ -299,10 +308,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,11 +326,11 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="n">
         <f aca="false">SUM(C4:C37)</f>
-        <v>55.5</v>
+        <v>58</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">C2*65</f>
-        <v>3607.5</v>
+        <v>3770</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +613,38 @@
         <v>32</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>4.5</v>
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
por fin el horizontal
</commit_message>
<xml_diff>
--- a/horas.xlsx
+++ b/horas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t xml:space="preserve">Fechas</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t xml:space="preserve">3-dic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-dic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">por fin hplstat</t>
   </si>
 </sst>
 </file>
@@ -233,12 +239,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -308,10 +314,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:G26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -326,11 +332,11 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="n">
         <f aca="false">SUM(C4:C37)</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">C2*65</f>
-        <v>3770</v>
+        <v>3900</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,6 +651,23 @@
       </c>
       <c r="D25" s="3" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
desde linuxel domingo noche
</commit_message>
<xml_diff>
--- a/horas.xlsx
+++ b/horas.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+  <si>
+    <t xml:space="preserve">Totales</t>
+  </si>
   <si>
     <t xml:space="preserve">Fechas</t>
   </si>
@@ -134,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">por fin hplstat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-dic</t>
   </si>
 </sst>
 </file>
@@ -144,13 +150,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD\-MMM"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -167,8 +172,92 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,12 +266,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -190,8 +321,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,13 +361,68 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,28 +439,45 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="23">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFF2F2F2"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -267,11 +485,11 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFF2F2F2"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -287,7 +505,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -314,10 +532,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G26"/>
+  <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -329,347 +547,381 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.53"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="0" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <f aca="false">SUM(C4:C37)</f>
-        <v>60</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <f aca="false">C2*65</f>
-        <v>3900</v>
+        <v>4095</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="n">
         <v>43765</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>43766</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>43766</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="n">
         <v>43767</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="n">
         <v>43768</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="n">
         <v>43769</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>9</v>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="n">
         <v>43770</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="n">
         <v>43771</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>43772</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>43775</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>43776</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="n">
-        <v>43772</v>
-      </c>
-      <c r="C13" s="3" t="n">
+      <c r="B16" s="3" t="n">
+        <v>43778</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>43779</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>43781</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>43783</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>43796</v>
+      </c>
+      <c r="C21" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>43775</v>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>43776</v>
-      </c>
-      <c r="C15" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>43778</v>
-      </c>
-      <c r="C16" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>43779</v>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>43781</v>
-      </c>
-      <c r="C18" s="3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>43783</v>
-      </c>
-      <c r="C19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="4" t="n">
-        <v>43796</v>
-      </c>
-      <c r="C21" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>28</v>
+      <c r="D21" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>28</v>
+      <c r="D22" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>28</v>
+      <c r="D23" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>28</v>
+      <c r="D24" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>28</v>
+      <c r="D26" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>